<commit_message>
changes for excel report message
</commit_message>
<xml_diff>
--- a/GenerateReport.xlsx
+++ b/GenerateReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>EMP ID</t>
   </si>
@@ -143,12 +143,17 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="00FF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,7 +169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
@@ -172,7 +177,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1:F11"/>
+  <dimension ref="B1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -192,135 +197,149 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="n">
-        <v>1001.0</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="n">
-        <v>1002.0</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="n">
-        <v>1003.0</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s" s="1">
-        <v>5</v>
-      </c>
-    </row>
     <row r="5">
-      <c r="B5" t="n">
-        <v>1004.0</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s" s="1">
-        <v>5</v>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="n">
-        <v>1005.0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
+        <v>1001.0</v>
+      </c>
+      <c r="C6"/>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="n">
-        <v>1006.0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
+        <v>1002.0</v>
+      </c>
+      <c r="C7"/>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="n">
-        <v>1007.0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
+        <v>1003.0</v>
+      </c>
+      <c r="C8"/>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="n">
-        <v>1008.0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
+        <v>1004.0</v>
+      </c>
+      <c r="C9"/>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="n">
-        <v>1009.0</v>
+        <v>1005.0</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="1">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="n">
+        <v>1006.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="n">
+        <v>1007.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="n">
+        <v>1008.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="n">
+        <v>1009.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="n">
         <v>1010.0</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s" s="1">
+      <c r="E15" t="s" s="1">
         <v>19</v>
       </c>
     </row>

</xml_diff>